<commit_message>
added 64 bit designs
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer64/30mhz/mxu_3x3/power.xlsx
+++ b/dtpu_configurations/only_integer64/30mhz/mxu_3x3/power.xlsx
@@ -128,7 +128,7 @@
     <col min="4" max="4" width="8.75" customWidth="true"/>
     <col min="5" max="5" width="8.75" customWidth="true"/>
     <col min="6" max="6" width="10.3125" customWidth="true"/>
-    <col min="7" max="7" width="10.3125" customWidth="true"/>
+    <col min="7" max="7" width="8.75" customWidth="true"/>
     <col min="8" max="8" width="10.3125" customWidth="true"/>
     <col min="9" max="9" width="8.75" customWidth="true"/>
     <col min="10" max="10" width="11.25" customWidth="true"/>
@@ -175,22 +175,22 @@
         <v>11</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>0.010991264134645462</v>
+        <v>0.015711084008216858</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.005536400713026524</v>
+        <v>0.005493159871548414</v>
       </c>
       <c r="D2" t="n" s="4">
-        <v>0.00393033679574728</v>
+        <v>0.0040701813995838165</v>
       </c>
       <c r="E2" t="n" s="4">
-        <v>0.0019886742811650038</v>
+        <v>0.003394484054297209</v>
       </c>
       <c r="F2" t="n" s="4">
-        <v>1.8136065591534134E-6</v>
+        <v>3.92246626290671E-8</v>
       </c>
       <c r="G2" t="n" s="4">
-        <v>6.485169869847596E-4</v>
+        <v>0.001065471675246954</v>
       </c>
       <c r="H2" t="n" s="4">
         <v>5.878788651898503E-4</v>
@@ -199,10 +199,10 @@
         <v>1.2575732469558716</v>
       </c>
       <c r="J2" t="n" s="4">
-        <v>0.125111922621727</v>
+        <v>0.12726984918117523</v>
       </c>
       <c r="K2" t="n" s="4">
-        <v>1.4063740968704224</v>
+        <v>1.415169358253479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>